<commit_message>
chore: update Excel template file
</commit_message>
<xml_diff>
--- a/config/template.xlsx
+++ b/config/template.xlsx
@@ -24,7 +24,7 @@
     <t>S.P.E 5.1.6 | OBRA NUEVA</t>
   </si>
   <si>
-    <t>MUNICIPALIDAD DE RECOLETA</t>
+    <t xml:space="preserve">MUNICIPALIDAD </t>
   </si>
   <si>
     <t>C</t>
@@ -98,7 +98,7 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Aptos Narrow"/>
+        <rFont val="Arial"/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -111,7 +111,7 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t>Párrafo 4.2 P.R.R.</t>
+      <t>Párrafo 4.2 P.R.C</t>
     </r>
   </si>
   <si>
@@ -136,7 +136,7 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Aptos Narrow"/>
+        <rFont val="Arial"/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -149,13 +149,13 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t>Art. 2.6.1 O.G.U.C. -  Art. 3.3.3 P.R.R.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Aptos Narrow"/>
+      <t>Art. 2.6.1 O.G.U.C. -  Art. 3.3.3 P.R.C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -168,13 +168,13 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t>Párrafo 4.3 P.R.R.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Aptos Narrow"/>
+      <t>Párrafo 4.3 P.R.C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -187,13 +187,13 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t>Párrafo 4.3 P.R.R.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Aptos Narrow"/>
+      <t>Párrafo 4.3 P.R.C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -206,13 +206,13 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t>Párrafo 4.3 P.R.R.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Aptos Narrow"/>
+      <t>Párrafo 4.3 P.R.C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -225,7 +225,7 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t>Párrafo 4.3 P.R.R.</t>
+      <t>Párrafo 4.3 P.R.C</t>
     </r>
   </si>
   <si>
@@ -234,7 +234,7 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Aptos Narrow"/>
+        <rFont val="Arial"/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -247,13 +247,13 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t>Párrafo 4.3 P.R.R.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Aptos Narrow"/>
+      <t>Párrafo 4.3 P.R.C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -266,7 +266,7 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t>Art. 2.6.2 O.G.U.C. -  Art. 3.3.4 P.R.R.</t>
+      <t>Art. 2.6.2 O.G.U.C. -  Art. 3.3.4 P.R.C</t>
     </r>
   </si>
   <si>
@@ -291,7 +291,7 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Aptos Narrow"/>
+        <rFont val="Arial"/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -304,13 +304,13 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t xml:space="preserve"> Art. 3.3.2 P.R.R.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Aptos Narrow"/>
+      <t xml:space="preserve"> Art. 3.3.2 P.R.C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -323,7 +323,7 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t>Art. 3.3.2 P.R.R.</t>
+      <t>Art. 3.3.2 P.R.C</t>
     </r>
   </si>
   <si>
@@ -367,7 +367,7 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Aptos Narrow"/>
+        <rFont val="Arial"/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -380,7 +380,7 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t xml:space="preserve"> Párrafo 5.2 P.R.R.</t>
+      <t xml:space="preserve"> Párrafo 5.2 P.R.C</t>
     </r>
   </si>
   <si>
@@ -405,7 +405,7 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Aptos Narrow"/>
+        <rFont val="Arial"/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -418,7 +418,7 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t>Párrafo 4.5 P.R.R.</t>
+      <t>Párrafo 4.5 P.R.C</t>
     </r>
   </si>
   <si>
@@ -1297,7 +1297,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1444,7 +1444,7 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="19" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="43" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1452,6 +1452,9 @@
     <xf borderId="44" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="19" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="19" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -1471,7 +1474,7 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="19" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="43" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -2056,7 +2059,7 @@
       <c r="F17" s="70"/>
       <c r="G17" s="70"/>
       <c r="H17" s="71"/>
-      <c r="I17" s="69"/>
+      <c r="I17" s="72"/>
       <c r="J17" s="33"/>
       <c r="K17" s="33"/>
       <c r="L17" s="13"/>
@@ -2065,7 +2068,7 @@
       <c r="A18" s="68">
         <v>2.0</v>
       </c>
-      <c r="B18" s="69" t="s">
+      <c r="B18" s="72" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="33"/>
@@ -2074,7 +2077,7 @@
       <c r="F18" s="70"/>
       <c r="G18" s="70"/>
       <c r="H18" s="71"/>
-      <c r="I18" s="72"/>
+      <c r="I18" s="73"/>
       <c r="J18" s="33"/>
       <c r="K18" s="33"/>
       <c r="L18" s="13"/>
@@ -2092,7 +2095,7 @@
       <c r="F19" s="70"/>
       <c r="G19" s="70"/>
       <c r="H19" s="71"/>
-      <c r="I19" s="69"/>
+      <c r="I19" s="72"/>
       <c r="J19" s="33"/>
       <c r="K19" s="33"/>
       <c r="L19" s="13"/>
@@ -2110,7 +2113,7 @@
       <c r="F20" s="70"/>
       <c r="G20" s="70"/>
       <c r="H20" s="71"/>
-      <c r="I20" s="73"/>
+      <c r="I20" s="74"/>
       <c r="J20" s="33"/>
       <c r="K20" s="33"/>
       <c r="L20" s="13"/>
@@ -2128,7 +2131,7 @@
       <c r="F21" s="70"/>
       <c r="G21" s="70"/>
       <c r="H21" s="71"/>
-      <c r="I21" s="73"/>
+      <c r="I21" s="74"/>
       <c r="J21" s="33"/>
       <c r="K21" s="33"/>
       <c r="L21" s="13"/>
@@ -2146,7 +2149,7 @@
       <c r="F22" s="70"/>
       <c r="G22" s="70"/>
       <c r="H22" s="71"/>
-      <c r="I22" s="73"/>
+      <c r="I22" s="74"/>
       <c r="J22" s="33"/>
       <c r="K22" s="33"/>
       <c r="L22" s="13"/>
@@ -2164,7 +2167,7 @@
       <c r="F23" s="70"/>
       <c r="G23" s="70"/>
       <c r="H23" s="71"/>
-      <c r="I23" s="72" t="s">
+      <c r="I23" s="73" t="s">
         <v>33</v>
       </c>
       <c r="J23" s="33"/>
@@ -2184,7 +2187,7 @@
       <c r="F24" s="70"/>
       <c r="G24" s="70"/>
       <c r="H24" s="71"/>
-      <c r="I24" s="69"/>
+      <c r="I24" s="72"/>
       <c r="J24" s="33"/>
       <c r="K24" s="33"/>
       <c r="L24" s="13"/>
@@ -2202,7 +2205,7 @@
       <c r="F25" s="70"/>
       <c r="G25" s="70"/>
       <c r="H25" s="71"/>
-      <c r="I25" s="74" t="s">
+      <c r="I25" s="75" t="s">
         <v>33</v>
       </c>
       <c r="J25" s="33"/>
@@ -2213,7 +2216,7 @@
       <c r="A26" s="68">
         <v>10.0</v>
       </c>
-      <c r="B26" s="69" t="s">
+      <c r="B26" s="72" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="33"/>
@@ -2222,7 +2225,7 @@
       <c r="F26" s="70"/>
       <c r="G26" s="70"/>
       <c r="H26" s="71"/>
-      <c r="I26" s="75"/>
+      <c r="I26" s="76"/>
       <c r="J26" s="33"/>
       <c r="K26" s="33"/>
       <c r="L26" s="13"/>
@@ -2240,7 +2243,7 @@
       <c r="F27" s="70"/>
       <c r="G27" s="70"/>
       <c r="H27" s="71"/>
-      <c r="I27" s="72"/>
+      <c r="I27" s="73"/>
       <c r="J27" s="33"/>
       <c r="K27" s="33"/>
       <c r="L27" s="13"/>
@@ -2258,7 +2261,7 @@
       <c r="F28" s="70"/>
       <c r="G28" s="70"/>
       <c r="H28" s="71"/>
-      <c r="I28" s="76" t="s">
+      <c r="I28" s="77" t="s">
         <v>33</v>
       </c>
       <c r="J28" s="33"/>
@@ -2269,7 +2272,7 @@
       <c r="A29" s="68">
         <v>13.0</v>
       </c>
-      <c r="B29" s="69" t="s">
+      <c r="B29" s="72" t="s">
         <v>39</v>
       </c>
       <c r="C29" s="33"/>
@@ -2278,7 +2281,7 @@
       <c r="F29" s="70"/>
       <c r="G29" s="70"/>
       <c r="H29" s="71"/>
-      <c r="I29" s="69"/>
+      <c r="I29" s="72"/>
       <c r="J29" s="33"/>
       <c r="K29" s="33"/>
       <c r="L29" s="13"/>
@@ -2287,7 +2290,7 @@
       <c r="A30" s="68">
         <v>14.0</v>
       </c>
-      <c r="B30" s="69" t="s">
+      <c r="B30" s="72" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="33"/>
@@ -2296,7 +2299,7 @@
       <c r="F30" s="70"/>
       <c r="G30" s="70"/>
       <c r="H30" s="71"/>
-      <c r="I30" s="76" t="s">
+      <c r="I30" s="77" t="s">
         <v>33</v>
       </c>
       <c r="J30" s="33"/>
@@ -2304,19 +2307,19 @@
       <c r="L30" s="13"/>
     </row>
     <row r="31" ht="18.0" customHeight="1">
-      <c r="A31" s="77">
+      <c r="A31" s="78">
         <v>15.0</v>
       </c>
-      <c r="B31" s="78" t="s">
+      <c r="B31" s="79" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="34"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="80"/>
-      <c r="I31" s="81"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="82"/>
       <c r="J31" s="33"/>
       <c r="K31" s="33"/>
       <c r="L31" s="13"/>
@@ -2325,7 +2328,7 @@
       <c r="A32" s="68">
         <v>16.0</v>
       </c>
-      <c r="B32" s="69" t="s">
+      <c r="B32" s="72" t="s">
         <v>42</v>
       </c>
       <c r="C32" s="33"/>
@@ -2334,7 +2337,7 @@
       <c r="F32" s="70"/>
       <c r="G32" s="70"/>
       <c r="H32" s="71"/>
-      <c r="I32" s="72"/>
+      <c r="I32" s="73"/>
       <c r="J32" s="33"/>
       <c r="K32" s="33"/>
       <c r="L32" s="13"/>
@@ -2352,7 +2355,7 @@
       <c r="F33" s="70"/>
       <c r="G33" s="70"/>
       <c r="H33" s="71"/>
-      <c r="I33" s="72" t="s">
+      <c r="I33" s="73" t="s">
         <v>33</v>
       </c>
       <c r="J33" s="33"/>
@@ -2360,41 +2363,41 @@
       <c r="L33" s="13"/>
     </row>
     <row r="34" ht="27.75" customHeight="1">
-      <c r="A34" s="82">
+      <c r="A34" s="83">
         <v>18.0</v>
       </c>
-      <c r="B34" s="83" t="s">
+      <c r="B34" s="84" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>
-      <c r="E34" s="84"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="86"/>
-      <c r="H34" s="87"/>
-      <c r="I34" s="88"/>
-      <c r="J34" s="88"/>
-      <c r="K34" s="88"/>
-      <c r="L34" s="89"/>
+      <c r="E34" s="85"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="88"/>
+      <c r="I34" s="89"/>
+      <c r="J34" s="89"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="90"/>
     </row>
     <row r="35" ht="27.0" customHeight="1">
-      <c r="A35" s="90" t="s">
+      <c r="A35" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="91"/>
-      <c r="C35" s="91"/>
-      <c r="D35" s="91"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="91"/>
-      <c r="G35" s="91"/>
-      <c r="H35" s="91"/>
-      <c r="I35" s="91"/>
-      <c r="J35" s="91"/>
-      <c r="K35" s="91"/>
+      <c r="B35" s="92"/>
+      <c r="C35" s="92"/>
+      <c r="D35" s="92"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="92"/>
+      <c r="G35" s="92"/>
+      <c r="H35" s="92"/>
+      <c r="I35" s="92"/>
+      <c r="J35" s="92"/>
+      <c r="K35" s="92"/>
       <c r="L35" s="10"/>
     </row>
     <row r="36" ht="28.5" customHeight="1">
-      <c r="A36" s="92" t="s">
+      <c r="A36" s="93" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="33"/>
@@ -2410,7 +2413,7 @@
       <c r="L36" s="13"/>
     </row>
     <row r="37" ht="30.0" customHeight="1">
-      <c r="A37" s="93" t="s">
+      <c r="A37" s="94" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="51"/>
@@ -2426,29 +2429,29 @@
       <c r="L37" s="16"/>
     </row>
     <row r="38" ht="28.5" customHeight="1">
-      <c r="A38" s="94" t="s">
+      <c r="A38" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="95"/>
-      <c r="C38" s="96"/>
-      <c r="D38" s="97" t="s">
+      <c r="B38" s="96"/>
+      <c r="C38" s="97"/>
+      <c r="D38" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="E38" s="95"/>
-      <c r="F38" s="95"/>
-      <c r="G38" s="98"/>
-      <c r="H38" s="99" t="s">
+      <c r="E38" s="96"/>
+      <c r="F38" s="96"/>
+      <c r="G38" s="99"/>
+      <c r="H38" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="I38" s="100"/>
-      <c r="J38" s="100"/>
-      <c r="K38" s="101"/>
-      <c r="L38" s="102" t="s">
+      <c r="I38" s="101"/>
+      <c r="J38" s="101"/>
+      <c r="K38" s="102"/>
+      <c r="L38" s="103" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="103"/>
+      <c r="A39" s="104"/>
       <c r="B39" s="57"/>
       <c r="C39" s="57"/>
       <c r="D39" s="57"/>
@@ -2462,7 +2465,7 @@
       <c r="L39" s="63"/>
     </row>
     <row r="40" ht="29.25" customHeight="1">
-      <c r="A40" s="104"/>
+      <c r="A40" s="105"/>
       <c r="B40" s="43"/>
       <c r="C40" s="43"/>
       <c r="D40" s="43"/>
@@ -2473,10 +2476,10 @@
       <c r="I40" s="43"/>
       <c r="J40" s="43"/>
       <c r="K40" s="43"/>
-      <c r="L40" s="105"/>
+      <c r="L40" s="106"/>
     </row>
     <row r="41" ht="27.0" customHeight="1">
-      <c r="A41" s="106" t="s">
+      <c r="A41" s="107" t="s">
         <v>50</v>
       </c>
       <c r="B41" s="51"/>

</xml_diff>